<commit_message>
chore: update images path on instances
</commit_message>
<xml_diff>
--- a/recordm/customUI/dash/assets/instances/DASHBOARD - SOLUTION.xlsx
+++ b/recordm/customUI/dash/assets/instances/DASHBOARD - SOLUTION.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mimes/.local/share/cob-cli/customize.dashboard.dash/recordm/customUI/dash/assets/instances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5436B138-2067-264D-BDFB-949E718C13DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130F491F-5F58-CE4A-AD68-D9B4D4C33FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="4700" windowWidth="27720" windowHeight="16300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5880" yWindow="4700" windowWidth="27720" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -172,7 +172,7 @@
     <t>/userm/#/user/q=FUNC {{arg}}</t>
   </si>
   <si>
-    <t>/recordm/localresource/dash/assets/improve.jpg</t>
+    <t>/recordm/localresource/dash/assets/images/improve.jpg</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -756,7 +758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>

</xml_diff>